<commit_message>
updated donor box list template with list of container profiles
</commit_message>
<xml_diff>
--- a/samples/Donor Box List Template.xlsx
+++ b/samples/Donor Box List Template.xlsx
@@ -10,7 +10,7 @@
     <sheet name="BOX LIST" sheetId="1" r:id="rId1"/>
     <sheet name="EXAMPLE" sheetId="6" r:id="rId2"/>
     <sheet name="EXPLANATION OF TERMS" sheetId="2" r:id="rId3"/>
-    <sheet name="Box Types" sheetId="5" r:id="rId4"/>
+    <sheet name="Container Profiles" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'BOX LIST'!$C$3:$H$41</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
   <si>
     <t>Box No</t>
   </si>
@@ -181,40 +181,88 @@
     <t>Box Type</t>
   </si>
   <si>
-    <t>Box Types</t>
-  </si>
-  <si>
-    <t>Box</t>
-  </si>
-  <si>
-    <t>Elephant-Folio</t>
-  </si>
-  <si>
-    <t>Folio</t>
-  </si>
-  <si>
-    <t>Folio-Box</t>
-  </si>
-  <si>
-    <t>Map-Folio</t>
-  </si>
-  <si>
-    <t>Piece</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
     <t>Album</t>
   </si>
   <si>
-    <t>Drawer</t>
-  </si>
-  <si>
-    <t>Folder</t>
-  </si>
-  <si>
-    <t>Negative box</t>
+    <t>Container Profiles</t>
+  </si>
+  <si>
+    <t>Box (Archives)</t>
+  </si>
+  <si>
+    <t>Box (Archives - Blue)</t>
+  </si>
+  <si>
+    <t>Box (MS)</t>
+  </si>
+  <si>
+    <t>Box (Object)</t>
+  </si>
+  <si>
+    <t>Box (Letter)</t>
+  </si>
+  <si>
+    <t>Phase Box (Small)</t>
+  </si>
+  <si>
+    <t>Phase Box (Medium)</t>
+  </si>
+  <si>
+    <t>Phase Box (Outsized)</t>
+  </si>
+  <si>
+    <t>Cassette Box</t>
+  </si>
+  <si>
+    <t>Folio Box (Small)</t>
+  </si>
+  <si>
+    <t>Folio Box (Medium)</t>
+  </si>
+  <si>
+    <t>Folio Box (Large)</t>
+  </si>
+  <si>
+    <t>Carton (Standard)</t>
+  </si>
+  <si>
+    <t>Carton (Outsized)</t>
+  </si>
+  <si>
+    <t>Negative Box</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Object (Small)</t>
+  </si>
+  <si>
+    <t>Object (Medium)</t>
+  </si>
+  <si>
+    <t>Object (Outsized)</t>
+  </si>
+  <si>
+    <t>Folio (Elephant)</t>
+  </si>
+  <si>
+    <t>Folio (Map)</t>
+  </si>
+  <si>
+    <t>Volume (Standard)</t>
+  </si>
+  <si>
+    <t>Volume (Large)</t>
+  </si>
+  <si>
+    <t>Security Binder</t>
+  </si>
+  <si>
+    <t>Binder (Pictures Blue)</t>
+  </si>
+  <si>
+    <t>Container Profile</t>
   </si>
 </sst>
 </file>
@@ -1167,13 +1215,13 @@
   <dimension ref="A1:H176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:H3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="12" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="30" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" style="31" customWidth="1"/>
     <col min="4" max="4" width="11.1640625" style="31" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" style="24" customWidth="1"/>
@@ -1232,7 +1280,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>0</v>
@@ -2624,7 +2672,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Box Types'!$B$4:$B$15</xm:f>
+            <xm:f>'Container Profiles'!$B$4:$B$30</xm:f>
           </x14:formula1>
           <xm:sqref>B5:B176</xm:sqref>
         </x14:dataValidation>
@@ -4167,7 +4215,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Box Types'!$B$4:$B$15</xm:f>
+            <xm:f>'Container Profiles'!$B$4:$B$15</xm:f>
           </x14:formula1>
           <xm:sqref>B5:B176</xm:sqref>
         </x14:dataValidation>
@@ -4381,7 +4429,7 @@
     <row r="3" spans="1:3" ht="36" customHeight="1">
       <c r="A3" s="41"/>
       <c r="B3" s="42" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="41"/>
     </row>
@@ -4392,153 +4440,183 @@
     <row r="5" spans="1:3" ht="18">
       <c r="A5" s="41"/>
       <c r="B5" s="43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="41"/>
     </row>
     <row r="6" spans="1:3" ht="18">
       <c r="A6" s="41"/>
       <c r="B6" s="43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" s="41"/>
     </row>
     <row r="7" spans="1:3" ht="18">
       <c r="A7" s="41"/>
       <c r="B7" s="43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" s="41"/>
     </row>
     <row r="8" spans="1:3" ht="18">
       <c r="A8" s="41"/>
       <c r="B8" s="43" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C8" s="41"/>
     </row>
     <row r="9" spans="1:3" ht="18">
       <c r="A9" s="41"/>
       <c r="B9" s="43" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="41"/>
     </row>
     <row r="10" spans="1:3" ht="18">
       <c r="A10" s="41"/>
       <c r="B10" s="43" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" s="41"/>
     </row>
     <row r="11" spans="1:3" ht="18">
       <c r="A11" s="41"/>
       <c r="B11" s="43" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C11" s="41"/>
     </row>
     <row r="12" spans="1:3" ht="18">
       <c r="A12" s="41"/>
       <c r="B12" s="43" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C12" s="41"/>
     </row>
     <row r="13" spans="1:3" ht="18">
       <c r="A13" s="41"/>
       <c r="B13" s="43" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C13" s="41"/>
     </row>
     <row r="14" spans="1:3" ht="18">
       <c r="A14" s="41"/>
       <c r="B14" s="43" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="41"/>
     </row>
     <row r="15" spans="1:3" ht="18">
       <c r="A15" s="41"/>
       <c r="B15" s="43" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="41"/>
     </row>
     <row r="16" spans="1:3" ht="18">
       <c r="A16" s="41"/>
-      <c r="B16" s="43"/>
+      <c r="B16" s="43" t="s">
+        <v>63</v>
+      </c>
       <c r="C16" s="41"/>
     </row>
     <row r="17" spans="1:3" ht="18">
       <c r="A17" s="41"/>
-      <c r="B17" s="43"/>
+      <c r="B17" s="43" t="s">
+        <v>64</v>
+      </c>
       <c r="C17" s="41"/>
     </row>
     <row r="18" spans="1:3" ht="18">
       <c r="A18" s="41"/>
-      <c r="B18" s="43"/>
+      <c r="B18" s="43" t="s">
+        <v>65</v>
+      </c>
       <c r="C18" s="41"/>
     </row>
     <row r="19" spans="1:3" ht="18">
       <c r="A19" s="41"/>
-      <c r="B19" s="43"/>
+      <c r="B19" s="43" t="s">
+        <v>50</v>
+      </c>
       <c r="C19" s="41"/>
     </row>
     <row r="20" spans="1:3" ht="18">
       <c r="A20" s="41"/>
-      <c r="B20" s="43"/>
+      <c r="B20" s="43" t="s">
+        <v>66</v>
+      </c>
       <c r="C20" s="41"/>
     </row>
     <row r="21" spans="1:3" ht="18">
       <c r="A21" s="41"/>
-      <c r="B21" s="43"/>
+      <c r="B21" s="43" t="s">
+        <v>67</v>
+      </c>
       <c r="C21" s="41"/>
     </row>
     <row r="22" spans="1:3" ht="18">
       <c r="A22" s="41"/>
-      <c r="B22" s="43"/>
+      <c r="B22" s="43" t="s">
+        <v>68</v>
+      </c>
       <c r="C22" s="41"/>
     </row>
     <row r="23" spans="1:3" ht="18">
       <c r="A23" s="41"/>
-      <c r="B23" s="43"/>
+      <c r="B23" s="43" t="s">
+        <v>69</v>
+      </c>
       <c r="C23" s="41"/>
     </row>
     <row r="24" spans="1:3" ht="18">
       <c r="A24" s="41"/>
-      <c r="B24" s="43"/>
+      <c r="B24" s="43" t="s">
+        <v>70</v>
+      </c>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:3" ht="18">
       <c r="A25" s="41"/>
-      <c r="B25" s="43"/>
+      <c r="B25" s="43" t="s">
+        <v>71</v>
+      </c>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:3" ht="18">
       <c r="A26" s="41"/>
-      <c r="B26" s="43"/>
+      <c r="B26" s="43" t="s">
+        <v>72</v>
+      </c>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:3" ht="18">
       <c r="A27" s="41"/>
-      <c r="B27" s="43"/>
+      <c r="B27" s="43" t="s">
+        <v>73</v>
+      </c>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:3" ht="18">
       <c r="A28" s="41"/>
-      <c r="B28" s="43"/>
+      <c r="B28" s="43" t="s">
+        <v>74</v>
+      </c>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:3" ht="18">
       <c r="A29" s="41"/>
-      <c r="B29" s="43"/>
+      <c r="B29" s="43" t="s">
+        <v>75</v>
+      </c>
       <c r="C29" s="41"/>
     </row>
     <row r="30" spans="1:3" ht="18">
       <c r="A30" s="41"/>
-      <c r="B30" s="43"/>
+      <c r="B30" s="43" t="s">
+        <v>76</v>
+      </c>
       <c r="C30" s="41"/>
     </row>
     <row r="31" spans="1:3" ht="18">

</xml_diff>

<commit_message>
updated names of Carton container profiles
</commit_message>
<xml_diff>
--- a/samples/Donor Box List Template.xlsx
+++ b/samples/Donor Box List Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26929"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="0" windowWidth="26080" windowHeight="14460"/>
+    <workbookView xWindow="460" yWindow="0" windowWidth="26080" windowHeight="14460" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BOX LIST" sheetId="1" r:id="rId1"/>
@@ -223,12 +223,6 @@
     <t>Folio Box (Large)</t>
   </si>
   <si>
-    <t>Carton (Standard)</t>
-  </si>
-  <si>
-    <t>Carton (Outsized)</t>
-  </si>
-  <si>
     <t>Negative Box</t>
   </si>
   <si>
@@ -263,6 +257,12 @@
   </si>
   <si>
     <t>Container Profile</t>
+  </si>
+  <si>
+    <t>Carton (MS)</t>
+  </si>
+  <si>
+    <t>Carton (Archives)</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1214,7 @@
   </sheetPr>
   <dimension ref="A1:H176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1280,7 +1280,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>0</v>
@@ -4404,8 +4404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4524,14 +4524,14 @@
     <row r="17" spans="1:3" ht="18">
       <c r="A17" s="41"/>
       <c r="B17" s="43" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C17" s="41"/>
     </row>
     <row r="18" spans="1:3" ht="18">
       <c r="A18" s="41"/>
       <c r="B18" s="43" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C18" s="41"/>
     </row>
@@ -4545,77 +4545,77 @@
     <row r="20" spans="1:3" ht="18">
       <c r="A20" s="41"/>
       <c r="B20" s="43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="41"/>
     </row>
     <row r="21" spans="1:3" ht="18">
       <c r="A21" s="41"/>
       <c r="B21" s="43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="41"/>
     </row>
     <row r="22" spans="1:3" ht="18">
       <c r="A22" s="41"/>
       <c r="B22" s="43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="41"/>
     </row>
     <row r="23" spans="1:3" ht="18">
       <c r="A23" s="41"/>
       <c r="B23" s="43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" s="41"/>
     </row>
     <row r="24" spans="1:3" ht="18">
       <c r="A24" s="41"/>
       <c r="B24" s="43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:3" ht="18">
       <c r="A25" s="41"/>
       <c r="B25" s="43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:3" ht="18">
       <c r="A26" s="41"/>
       <c r="B26" s="43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:3" ht="18">
       <c r="A27" s="41"/>
       <c r="B27" s="43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:3" ht="18">
       <c r="A28" s="41"/>
       <c r="B28" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:3" ht="18">
       <c r="A29" s="41"/>
       <c r="B29" s="43" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" s="41"/>
     </row>
     <row r="30" spans="1:3" ht="18">
       <c r="A30" s="41"/>
       <c r="B30" s="43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="41"/>
     </row>

</xml_diff>